<commit_message>
huge improve and debug
</commit_message>
<xml_diff>
--- a/Attendance.Web/Files/drivers.xlsx
+++ b/Attendance.Web/Files/drivers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zavosh1010\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkPlace\Attendance\Attendance.Web\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>FirstName</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>کریمی</t>
+  </si>
+  <si>
+    <t>Birthdate</t>
+  </si>
+  <si>
+    <t>1378/06/13</t>
   </si>
 </sst>
 </file>
@@ -359,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -370,7 +376,7 @@
     <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,8 +389,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -396,6 +405,9 @@
       </c>
       <c r="D2">
         <v>9483473483</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>